<commit_message>
message: journal-entry problem solved and chequeNo update problem solved and manual changes of product(add maxSaleQty,notForSale,bestBefore,cess) completed
</commit_message>
<xml_diff>
--- a/public/Documents/NewApiDoc(6-10).xlsx
+++ b/public/Documents/NewApiDoc(6-10).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1946" uniqueCount="1468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="1491">
   <si>
     <t>Laravel Api(06-10-2016)               @Virat Sir</t>
   </si>
@@ -7125,6 +7125,75 @@
   </si>
   <si>
     <t>app\views\QuickMenu\RetailsaleBill.html</t>
+  </si>
+  <si>
+    <t>analysis arihant task and somewhat discuss with jigar sir</t>
+  </si>
+  <si>
+    <t>merge all changes of arihant with erp except template color change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- front-end github push(not working)</t>
+  </si>
+  <si>
+    <t>Extra-Work</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- sidebar &gt;&gt; if user is staff then cant click on add/edit staff</t>
+  </si>
+  <si>
+    <t>SettingController.php</t>
+  </si>
+  <si>
+    <t>Back-End(arihant done)</t>
+  </si>
+  <si>
+    <t>problem solved of journal-entry &gt;&gt; amount calculation result  is = -0.00400000000002(bz of not converting data to decimal_points)</t>
+  </si>
+  <si>
+    <t>billprocessor.php</t>
+  </si>
+  <si>
+    <t>problem solved of chequeNo update &gt;&gt; when chequeno status off from settings</t>
+  </si>
+  <si>
+    <t>upload to arihant,silicon &amp; swaminarayan server and testing</t>
+  </si>
+  <si>
+    <t>upload to arihant and testing properly</t>
+  </si>
+  <si>
+    <t>Hint :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> product changes shpuld be in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- product model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- product display page</t>
+  </si>
+  <si>
+    <t>Product Change : (Add Field &gt;&gt; maxSaleQty,notForSale,bestBefore,cess)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- View Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- product api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -- add product api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -- update product api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -- get single &amp; multiple data api</t>
   </si>
 </sst>
 </file>
@@ -10328,10 +10397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1092"/>
+  <dimension ref="A1:I1129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1078" workbookViewId="0">
-      <selection activeCell="C1093" sqref="C1093"/>
+    <sheetView tabSelected="1" topLeftCell="A1096" workbookViewId="0">
+      <selection activeCell="C1111" sqref="C1111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16752,6 +16821,166 @@
     <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1092" t="s">
         <v>1375</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1094" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1095" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1096" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1097" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1098" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1099" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1100" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1101" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1102" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1103" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1104" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="1105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1105" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="1106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1106" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1107" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1108" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="1109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1109" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="1110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1110" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="1111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1111" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="1113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1113" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1114" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="1119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1119" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1120" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="1122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1122" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="1123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1123" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="1125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1125" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="1126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1126" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="1127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1127" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="1128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1128" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="1129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1129" t="s">
+        <v>1484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
message: manual changes of setting api completed(add product color,size,bestBefore)
</commit_message>
<xml_diff>
--- a/public/Documents/NewApiDoc(6-10).xlsx
+++ b/public/Documents/NewApiDoc(6-10).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="1491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1497">
   <si>
     <t>Laravel Api(06-10-2016)               @Virat Sir</t>
   </si>
@@ -7194,6 +7194,24 @@
   </si>
   <si>
     <t xml:space="preserve">      -- get single &amp; multiple data api</t>
+  </si>
+  <si>
+    <t>Git push</t>
+  </si>
+  <si>
+    <t>Asana Task Updating In Arihant</t>
+  </si>
+  <si>
+    <t>Setting Api Change (Add bestBefore &amp; color-size setting in product)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Design Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- get,set,add,update data add/set in formdata/form</t>
   </si>
 </sst>
 </file>
@@ -10397,9 +10415,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1129"/>
+  <dimension ref="A1:I1134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1096" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1104" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1111" sqref="C1111"/>
     </sheetView>
   </sheetViews>
@@ -16895,92 +16913,137 @@
     </row>
     <row r="1105" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1105" t="s">
-        <v>1053</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1106" t="s">
-        <v>990</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="1107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1107" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="1108" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1108" t="s">
-        <v>1487</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1109" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1109" t="s">
-        <v>1488</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="1110" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1110" t="s">
-        <v>1489</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1111" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1111" t="s">
-        <v>1490</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1113" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1113" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="1114" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1114" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1115" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1116" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1117" t="s">
         <v>1486</v>
+      </c>
+    </row>
+    <row r="1118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1118" t="s">
+        <v>1492</v>
       </c>
     </row>
     <row r="1119" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1119" t="s">
-        <v>432</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1120" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1120" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1121" t="s">
         <v>1470</v>
-      </c>
-    </row>
-    <row r="1122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1122" t="s">
-        <v>1471</v>
       </c>
     </row>
     <row r="1123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1123" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="1124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1124" t="s">
         <v>1472</v>
-      </c>
-    </row>
-    <row r="1125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1125" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="1126" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1126" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1127" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1128" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1129" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="1130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1130" t="s">
         <v>1484</v>
+      </c>
+    </row>
+    <row r="1131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1131" s="47" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="1132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1132" s="47" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="1133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1133" s="47" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="1134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1134" s="47" t="s">
+        <v>1490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
message: setting api changes for adding product setting completer
</commit_message>
<xml_diff>
--- a/public/Documents/NewApiDoc(6-10).xlsx
+++ b/public/Documents/NewApiDoc(6-10).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="1502">
   <si>
     <t>Laravel Api(06-10-2016)               @Virat Sir</t>
   </si>
@@ -7205,13 +7205,28 @@
     <t>Setting Api Change (Add bestBefore &amp; color-size setting in product)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -- api changes</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -- Design Changes</t>
   </si>
   <si>
-    <t xml:space="preserve"> -- get,set,add,update data add/set in formdata/form</t>
+    <t>Setting Api</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- insert api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- update api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- get all data &amp; get particular api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- get data and set data to form</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- insert/update data set to form-data(only once insert then update)</t>
+  </si>
+  <si>
+    <t>Product Api Changes</t>
   </si>
 </sst>
 </file>
@@ -10415,10 +10430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1134"/>
+  <dimension ref="A1:I1138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1111" sqref="C1111"/>
+    <sheetView tabSelected="1" topLeftCell="A1105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1116" sqref="C1116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16819,8 +16834,8 @@
       <c r="C1089" t="s">
         <v>1462</v>
       </c>
-      <c r="D1089" s="64" t="s">
-        <v>1105</v>
+      <c r="D1089" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
@@ -16828,39 +16843,50 @@
         <v>1466</v>
       </c>
       <c r="D1090" s="64" t="s">
-        <v>1467</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1091" t="s">
         <v>1465</v>
       </c>
+      <c r="D1091" s="64" t="s">
+        <v>1467</v>
+      </c>
     </row>
     <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1092" t="s">
         <v>1375</v>
       </c>
+      <c r="D1092" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1093" t="s">
+        <v>1333</v>
+      </c>
     </row>
     <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1094" t="s">
         <v>1468</v>
       </c>
+      <c r="D1094" t="s">
+        <v>1399</v>
+      </c>
     </row>
     <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1095" t="s">
         <v>1469</v>
       </c>
       <c r="D1095" t="s">
-        <v>1332</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1096" t="s">
         <v>1479</v>
       </c>
-      <c r="D1096" t="s">
-        <v>1333</v>
-      </c>
     </row>
     <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1097" t="s">
@@ -16910,139 +16936,165 @@
       <c r="C1104" t="s">
         <v>1485</v>
       </c>
-    </row>
-    <row r="1105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D1104" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="1105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1105" t="s">
         <v>1493</v>
       </c>
-    </row>
-    <row r="1106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="D1105" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1106" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="1107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="1107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1107" t="s">
         <v>990</v>
       </c>
     </row>
-    <row r="1108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="1108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1108" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="1109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1109" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="1110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1110" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="1111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1111" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1112" t="s">
         <v>1494</v>
       </c>
     </row>
-    <row r="1109" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1109" t="s">
+    <row r="1113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1113" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="1114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1114" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="1116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1116" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="1117" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1117" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="1118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1118" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1119" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1120" t="s">
         <v>1052</v>
-      </c>
-    </row>
-    <row r="1110" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1110" t="s">
-        <v>1495</v>
-      </c>
-    </row>
-    <row r="1111" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1111" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="1113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1113" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="1114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1114" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="1115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1115" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="1116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1116" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="1117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1117" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="1118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1118" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="1119" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1119" t="s">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="1120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1120" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="1121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1121" t="s">
-        <v>1470</v>
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="1122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1122" t="s">
+        <v>1492</v>
       </c>
     </row>
     <row r="1123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1123" t="s">
-        <v>1471</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1124" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1124" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="1126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1126" t="s">
-        <v>1480</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1125" t="s">
+        <v>1470</v>
       </c>
     </row>
     <row r="1127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1127" t="s">
-        <v>1481</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1128" t="s">
-        <v>1482</v>
-      </c>
-    </row>
-    <row r="1129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1129" t="s">
-        <v>1483</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1130" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="1131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1131" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="1132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1132" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="1133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1133" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="1134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1134" t="s">
         <v>1484</v>
       </c>
     </row>
-    <row r="1131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1131" s="47" t="s">
+    <row r="1135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1135" s="47" t="s">
         <v>1487</v>
       </c>
     </row>
-    <row r="1132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1132" s="47" t="s">
+    <row r="1136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1136" s="47" t="s">
         <v>1488</v>
       </c>
     </row>
-    <row r="1133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1133" s="47" t="s">
+    <row r="1137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1137" s="47" t="s">
         <v>1489</v>
       </c>
     </row>
-    <row r="1134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1134" s="47" t="s">
+    <row r="1138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1138" s="47" t="s">
         <v>1490</v>
       </c>
     </row>

</xml_diff>

<commit_message>
message: bill update problem solve and bill get all data with full company detail completed
</commit_message>
<xml_diff>
--- a/public/Documents/NewApiDoc(6-10).xlsx
+++ b/public/Documents/NewApiDoc(6-10).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="2014">
   <si>
     <t>Laravel Api(06-10-2016)               @Virat Sir</t>
   </si>
@@ -6756,9 +6756,6 @@
     <t>uploading all on silicon server-swaminarayan and testing it with cron-job background process till date:12-feb-2018</t>
   </si>
   <si>
-    <t>silicon uploading : yellow,swaminarayan uploading : Orange,arihant uploading : green</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -- service date default setting problem &gt;&gt; solved</t>
   </si>
   <si>
@@ -8495,9 +8492,6 @@
     <t xml:space="preserve"> templateDesign.php</t>
   </si>
   <si>
-    <t xml:space="preserve"> swaminarayan and arihant done</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Uploading on swaminarayan &amp; arihant server and testing on it</t>
   </si>
   <si>
@@ -8516,9 +8510,6 @@
     <t xml:space="preserve"> local testing and uploading on server with testing</t>
   </si>
   <si>
-    <t>api</t>
-  </si>
-  <si>
     <t xml:space="preserve"> messagecontroller.php</t>
   </si>
   <si>
@@ -8540,9 +8531,6 @@
     <t xml:space="preserve"> -- server loading problem &gt;&gt; FTp and site is not loading</t>
   </si>
   <si>
-    <t xml:space="preserve"> arihant-swaminarayan done</t>
-  </si>
-  <si>
     <t xml:space="preserve"> cess is not working in product</t>
   </si>
   <si>
@@ -8610,6 +8598,182 @@
   </si>
   <si>
     <t xml:space="preserve">     -- show-hide data as per setting and adjust design of bill</t>
+  </si>
+  <si>
+    <t>constant.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> problem solve of not sending message to parent and teacher from api to web</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> generate an excel of product-data(id,name,category_id,category_name,group_id,group_name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> problem solve of pragnesh &gt;&gt; sending message/notification to all student,all parent,all teacher,all student of school,all parent of school,all teacher of school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Description :</t>
+  </si>
+  <si>
+    <t>problem : cant send Message From web to app -- actually properly message is send from web to app..                                                                                                                                                        which is display in web inbox -- but send message is not display in app inbox -- find the problem and try to solve this problem                                                                                                        -- here message sending possibilities are more..like...all students,all student of school,particular students,parents etc...                                                                                                                               -- change the api for getting inbox data -- currently we found the problem in display data in app inbox...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solve the problem of not displaying name in web inbox &gt;&gt; problem occur when message is send from app to web</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- found that the database have no name in that case..thats why not displaying name in web inbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> changes &gt;&gt; when settings for city-state is disable &gt;&gt; not set the default value in database..</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- testing from various side ... can we display state-city properly or not??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -- database(table-name: ledger,client) changes of setting null as a default value in state-city</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> git &gt;&gt; cant switch from one user to another(use : git config --global user.name "fshaikhsb" )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Replace Caption in Quick Access Tax Invoice Tax Purchase To Sale Invoice &amp; Purchase</t>
+  </si>
+  <si>
+    <t>app\views\Accounting\viewData\AccDataViews.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dynamic company logo display completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -- Working on Display Logo with company name</t>
+  </si>
+  <si>
+    <t>Replace Some Filed In Accounting &gt;&gt; sales</t>
+  </si>
+  <si>
+    <t>Replace Perticular  with Client Name
+Marge Debit &amp; Credit to Debit/credit
+Add New Filed Amount</t>
+  </si>
+  <si>
+    <t>app\views\Company\AddCompany.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> image upload conpression(with quality/ only size)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Image display in product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> preprint problem of sanjaybhai</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In sales bill view Replace TYPE value of Retail Sales,Whole Sales to Cash credit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Replace Color &amp; Size with Base unit &amp; secondary Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> git problem</t>
+  </si>
+  <si>
+    <t>app\js\controllers\Company\AddCompanyCtrl.js</t>
+  </si>
+  <si>
+    <t>Try to compress and set image (image is compressed but it is streched)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> on image update &gt;&gt; set logo on top-bar</t>
+  </si>
+  <si>
+    <t>app\views\Company\Company.html</t>
+  </si>
+  <si>
+    <t>app\js\controllers\Company\CompanyCtrl.js</t>
+  </si>
+  <si>
+    <t>In sales bill view Replace TYPE value of Retail Sales,Whole Sales to Cash credit</t>
+  </si>
+  <si>
+    <t>smartclass api</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uploading to server of arihant,swaminarayan and testing properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silicon uploading : yellow,swaminarayan uploading : Orange,arihant uploading : green ,all uploading: blue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> js change(add folder image-compress &gt;&gt; app/js/customJS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- database changes and uploading front-back side file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- problem solve &gt;&gt; when frame-no is disabled &gt;&gt; design of product table in bill is changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     same problem solution is implement in purchase-bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Back-End( arihant-swaminarayan done)</t>
+  </si>
+  <si>
+    <t>DB Changes(arihant-swaminarayan done)</t>
+  </si>
+  <si>
+    <t>Front-end(arihant-swaminarayan done)</t>
+  </si>
+  <si>
+    <t>Front-End(arihant-swaminarayan done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Front-End(arihant-swaminarayan done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Back-End(swaminarayan and arihant done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Server uploading  testing completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- preprint somewhat design problem solve by calling client and testing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     -- this problem is not occur with our printer bz the page size of our and client is different</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- problem solve &gt;&gt; after saving a particular bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     -- when we click on previous button &gt;&gt; it always print printed bill (not preprint bill as per setting) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- problem solve : sometime discount and amount field size becomes bigger than others</t>
+  </si>
+  <si>
+    <t>app\Core\Accounting\Bills\Entities\EncodeAllData.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- problem solve : after click on previous button in bill &gt;&gt; click on print &gt;&gt; cant open bill with print screen(asks for change the data)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> updating all completed task on asana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solve the git problem(farhan is not added to team in github)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> igst problem state-city wise</t>
+  </si>
+  <si>
+    <t>Front-End(swaminarayan done)</t>
+  </si>
+  <si>
+    <t>Back-End(swaminarayan done)</t>
   </si>
 </sst>
 </file>
@@ -11849,10 +12013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1668"/>
+  <dimension ref="A1:I1715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1648" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1668" sqref="C1668"/>
+    <sheetView tabSelected="1" topLeftCell="B1701" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1705" sqref="D1705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11890,7 +12054,7 @@
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="C4" s="37" t="s">
-        <v>1346</v>
+        <v>1990</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="25"/>
@@ -17253,7 +17417,7 @@
     </row>
     <row r="907" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C907" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="910" spans="1:4" x14ac:dyDescent="0.25">
@@ -17547,7 +17711,7 @@
         <v>1339</v>
       </c>
       <c r="D957" s="64" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="958" spans="1:4" x14ac:dyDescent="0.25">
@@ -17573,42 +17737,42 @@
     </row>
     <row r="961" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C961" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="962" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C962" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="963" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C963" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="964" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C964" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="965" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C965" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="966" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C966" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="967" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C967" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="968" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C968" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D968" s="64" t="s">
         <v>1223</v>
@@ -17616,22 +17780,22 @@
     </row>
     <row r="969" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C969" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="970" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C970" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="971" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C971" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="972" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C972" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="973" spans="3:4" x14ac:dyDescent="0.25">
@@ -17641,27 +17805,27 @@
     </row>
     <row r="974" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C974" s="10" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="975" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C975" s="10" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="976" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C976" s="7" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="977" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C977" s="10" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="978" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C978" s="10" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="981" spans="1:4" x14ac:dyDescent="0.25">
@@ -17672,7 +17836,7 @@
         <v>1263</v>
       </c>
       <c r="C981" s="10" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D981" t="s">
         <v>1053</v>
@@ -17680,51 +17844,51 @@
     </row>
     <row r="982" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C982" s="10" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D982" s="64" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="983" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C983" s="10" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D983" s="64" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="984" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D984" s="64" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="985" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C985" s="10" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="D985" s="64" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="986" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C986" s="10" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="987" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C987" s="10" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="988" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C988" s="10" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="990" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C990" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="D990" t="s">
         <v>1052</v>
@@ -17732,10 +17896,10 @@
     </row>
     <row r="991" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C991" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D991" s="64" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="992" spans="1:4" x14ac:dyDescent="0.25">
@@ -17758,68 +17922,68 @@
         <v>43146</v>
       </c>
       <c r="B996" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="997" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C997" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="998" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C998" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="999" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C999" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1000" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1000" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1001" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1001" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1002" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1002" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="D1002" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1003" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1003" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="D1003" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1004" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1004" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1005" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1005" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1006" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C1006" s="3" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1007" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1007" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1010" spans="2:4" x14ac:dyDescent="0.25">
@@ -17827,7 +17991,7 @@
         <v>568</v>
       </c>
       <c r="C1010" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="D1010" t="s">
         <v>1052</v>
@@ -17835,15 +17999,15 @@
     </row>
     <row r="1011" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1011" s="64" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1012" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1012" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="D1012" s="64" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1013" spans="2:4" x14ac:dyDescent="0.25">
@@ -17856,7 +18020,7 @@
     </row>
     <row r="1014" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1014" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="D1014" s="64" t="s">
         <v>1206</v>
@@ -17864,70 +18028,70 @@
     </row>
     <row r="1015" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1015" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1016" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1016" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D1016" s="64" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1017" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1017" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D1017" s="64" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1018" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1018" s="10" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="D1018" s="64" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1019" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1019" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="D1019" s="64" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1020" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1020" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="D1020" s="64" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1021" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1021" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="D1021" s="64" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1022" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1022" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1023" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1023" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1024" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1024" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="D1024" t="s">
         <v>1053</v>
@@ -17935,51 +18099,51 @@
     </row>
     <row r="1025" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1025" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D1025" s="64" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1026" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1026" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="D1026" s="64" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="1027" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1027" s="10" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="D1027" s="64" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1033" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1033" s="65" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1034" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1034" s="10" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="1035" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1035" s="10" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1036" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1036" s="10" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="1037" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1037" s="10" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="1038" spans="1:4" x14ac:dyDescent="0.25">
@@ -17989,14 +18153,14 @@
     </row>
     <row r="1039" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1039" s="10" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1040" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1040" s="70"/>
       <c r="B1040" s="70"/>
       <c r="C1040" s="71" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="D1040" s="70"/>
     </row>
@@ -18008,7 +18172,7 @@
         <v>1263</v>
       </c>
       <c r="C1042" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="D1042" t="s">
         <v>1053</v>
@@ -18016,70 +18180,70 @@
     </row>
     <row r="1043" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1043" s="10" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D1043" s="64" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1044" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1044" s="10" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D1044" s="64" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="1045" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1045" s="10" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D1045" s="64" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1046" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1046" s="10" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D1046" s="64" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1047" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1047" s="10" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D1047" s="64" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1048" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1048" s="10" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D1048" s="64" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1049" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1049" s="10" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="1050" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1050" s="10" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="1051" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1051" s="10" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="1052" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1052" s="10" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1053" spans="1:4" x14ac:dyDescent="0.25">
@@ -18089,23 +18253,23 @@
     </row>
     <row r="1054" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1054" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1055" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1055" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="C1055" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D1055" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1056" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1056" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="D1056" s="64" t="s">
         <v>1222</v>
@@ -18113,7 +18277,7 @@
     </row>
     <row r="1057" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1057" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D1057" t="s">
         <v>1342</v>
@@ -18121,7 +18285,7 @@
     </row>
     <row r="1058" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1058" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="D1058" s="64" t="s">
         <v>1183</v>
@@ -18129,17 +18293,17 @@
     </row>
     <row r="1059" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1059" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="1060" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1060" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="1061" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1061" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="1063" spans="2:4" x14ac:dyDescent="0.25">
@@ -18147,27 +18311,27 @@
         <v>568</v>
       </c>
       <c r="C1063" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1064" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1064" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="1065" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1065" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="1067" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1067" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="1068" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1068" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="D1068" s="64" t="s">
         <v>856</v>
@@ -18175,12 +18339,12 @@
     </row>
     <row r="1069" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1069" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1070" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1070" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1073" spans="1:4" x14ac:dyDescent="0.25">
@@ -18191,17 +18355,17 @@
         <v>1263</v>
       </c>
       <c r="C1073" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1074" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1074" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1075" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1075" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="1079" spans="1:4" x14ac:dyDescent="0.25">
@@ -18214,7 +18378,7 @@
     </row>
     <row r="1080" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1080" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="D1080" s="64" t="s">
         <v>1050</v>
@@ -18222,7 +18386,7 @@
     </row>
     <row r="1081" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1081" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="D1081" s="64" t="s">
         <v>1325</v>
@@ -18230,17 +18394,17 @@
     </row>
     <row r="1082" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1082" s="64" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1083" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1083" s="64" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1084" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1084" s="64" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1087" spans="1:4" x14ac:dyDescent="0.25">
@@ -18259,7 +18423,7 @@
         <v>1263</v>
       </c>
       <c r="C1089" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D1089" t="s">
         <v>1052</v>
@@ -18267,7 +18431,7 @@
     </row>
     <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1090" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="D1090" s="64" t="s">
         <v>1105</v>
@@ -18275,15 +18439,15 @@
     </row>
     <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1091" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="D1091" s="64" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1092" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D1092" s="68" t="s">
         <v>1332</v>
@@ -18296,23 +18460,23 @@
     </row>
     <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1094" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="D1094" s="68" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1095" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="D1095" s="68" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1096" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
@@ -18332,47 +18496,47 @@
     </row>
     <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1100" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="D1100" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1101" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="D1101" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1102" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D1102" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1103" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1104" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="D1104" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="1105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1105" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="D1105" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1106" spans="3:4" x14ac:dyDescent="0.25">
@@ -18387,17 +18551,17 @@
     </row>
     <row r="1108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1108" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="1109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1109" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="1110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1110" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="1111" spans="3:4" x14ac:dyDescent="0.25">
@@ -18407,22 +18571,22 @@
     </row>
     <row r="1112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1112" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="1113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1113" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="1114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1114" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="1116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1116" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="1117" spans="3:4" x14ac:dyDescent="0.25">
@@ -18447,17 +18611,17 @@
     </row>
     <row r="1121" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1121" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="1122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1122" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="1123" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1123" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="1124" spans="3:3" x14ac:dyDescent="0.25">
@@ -18467,62 +18631,62 @@
     </row>
     <row r="1125" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1125" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="1127" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1127" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="1128" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1128" s="7" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1130" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="1131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1131" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="1132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1132" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="1133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1133" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="1134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1134" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="1135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1135" s="47" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1136" s="47" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="1137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1137" s="47" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="1138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1138" s="47" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="1141" spans="1:4" x14ac:dyDescent="0.25">
@@ -18530,167 +18694,167 @@
         <v>43151</v>
       </c>
       <c r="B1141" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C1141" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D1141" t="s">
         <v>1502</v>
-      </c>
-      <c r="C1141" t="s">
-        <v>1506</v>
-      </c>
-      <c r="D1141" t="s">
-        <v>1503</v>
       </c>
     </row>
     <row r="1142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1142" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D1142" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1143" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D1143" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1144" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1145" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="1146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1146" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="1147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1147" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="1148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1148" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="1149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1149" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1150" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1151" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1152" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1153" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1154" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1155" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1156" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1157" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1158" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1159" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1161" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1162" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1163" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1165" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="C1165" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1166" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1167" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C1168" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1169" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1170" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1171" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1173" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="D1173" t="s">
         <v>1052</v>
@@ -18698,18 +18862,18 @@
     </row>
     <row r="1174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1174" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D1174" s="64" t="s">
         <v>1536</v>
-      </c>
-      <c r="D1174" s="64" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="1175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1175" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D1175" s="64" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1177" spans="1:4" x14ac:dyDescent="0.25">
@@ -18717,122 +18881,122 @@
         <v>43152</v>
       </c>
       <c r="C1177" s="47" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1178" s="47" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1179" s="47" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1180" s="47" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1181" s="47" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1182" s="47" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1183" s="47" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1184" s="47" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1185" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1185" s="47" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="1186" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1186" s="47" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1188" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1188" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1189" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1189" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1190" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1190" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="1191" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1191" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1192" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1192" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1193" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1193" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="1194" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1194" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="1195" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1195" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1196" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1196" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="1197" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1197" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="1198" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1198" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="1199" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1199" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="1200" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1200" s="47" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="1201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1201" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="1204" spans="1:4" x14ac:dyDescent="0.25">
@@ -18840,10 +19004,10 @@
         <v>43153</v>
       </c>
       <c r="B1204" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C1204" t="s">
         <v>1563</v>
-      </c>
-      <c r="C1204" t="s">
-        <v>1564</v>
       </c>
       <c r="D1204" t="s">
         <v>1052</v>
@@ -18851,7 +19015,7 @@
     </row>
     <row r="1205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1205" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D1205" s="64" t="s">
         <v>1332</v>
@@ -18859,7 +19023,7 @@
     </row>
     <row r="1206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1206" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="D1206" s="64" t="s">
         <v>1333</v>
@@ -18867,7 +19031,7 @@
     </row>
     <row r="1207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1207" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="D1207" s="64" t="s">
         <v>1325</v>
@@ -18875,94 +19039,94 @@
     </row>
     <row r="1208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1208" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="D1208" s="64" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="1209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1209" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D1209" s="64" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="1210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1210" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D1210" s="64" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="1211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1211" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D1211" s="64" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1212" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D1212" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1213" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D1213" s="64" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1214" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D1214" s="64" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1215" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D1215" s="64" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="1216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1216" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D1216" s="64" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1217" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1218" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="1219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1219" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="1220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1220" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="D1220" t="s">
         <v>1053</v>
@@ -18970,31 +19134,31 @@
     </row>
     <row r="1221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1221" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="D1221" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1222" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D1222" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="1223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1223" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="1224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1224" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D1224" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1225" spans="2:4" x14ac:dyDescent="0.25">
@@ -19002,7 +19166,7 @@
         <v>990</v>
       </c>
       <c r="D1225" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1226" spans="2:4" x14ac:dyDescent="0.25">
@@ -19012,12 +19176,12 @@
     </row>
     <row r="1227" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1227" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="1228" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1228" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="1231" spans="2:4" x14ac:dyDescent="0.25">
@@ -19025,62 +19189,62 @@
         <v>1342</v>
       </c>
       <c r="C1231" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="1232" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1232" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="1234" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1234" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1235" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1235" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="1245" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1245" s="47" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1246" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1246" s="47" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="1249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1249" s="47" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="1250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1250" s="47" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1251" s="47" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1252" s="47" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="1253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1253" s="47" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="1254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1254" s="47" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="1257" spans="1:4" x14ac:dyDescent="0.25">
@@ -19088,10 +19252,10 @@
         <v>43154</v>
       </c>
       <c r="B1257" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C1257" s="10" t="s">
         <v>1607</v>
-      </c>
-      <c r="C1257" s="10" t="s">
-        <v>1608</v>
       </c>
       <c r="D1257" t="s">
         <v>1052</v>
@@ -19107,7 +19271,7 @@
     </row>
     <row r="1259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1259" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D1259" s="64" t="s">
         <v>1333</v>
@@ -19115,45 +19279,45 @@
     </row>
     <row r="1260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1260" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D1260" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1261" s="10" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1262" s="10" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1263" s="10" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1264" s="10" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1265" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1265" s="10" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1266" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1266" s="10" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1267" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1267" s="10" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="D1267" t="s">
         <v>1053</v>
@@ -19161,7 +19325,7 @@
     </row>
     <row r="1268" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1268" s="10" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1269" spans="3:4" x14ac:dyDescent="0.25">
@@ -19169,133 +19333,133 @@
         <v>1053</v>
       </c>
       <c r="D1269" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="1270" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1270" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D1270" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="1271" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1271" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="D1271" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="1272" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1272" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="1273" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1273" s="10" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1274" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1274" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="1275" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1275" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="1276" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1276" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="1277" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1277" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1278" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1278" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="1279" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1279" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1280" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1280" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="1281" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1281" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="1283" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1283" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="1284" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1284" s="45" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1286" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1286" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="1287" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1287" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="1288" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1288" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1289" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1289" s="47" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="1290" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1290" s="47" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="1291" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1291" s="47" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="1292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1292" s="47" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1293" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1293" s="47" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="1294" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1294" s="47" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="1295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1295" s="47" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="1298" spans="1:4" x14ac:dyDescent="0.25">
@@ -19303,7 +19467,7 @@
         <v>43155</v>
       </c>
       <c r="C1298" s="10" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D1298" t="s">
         <v>1052</v>
@@ -19314,44 +19478,44 @@
         <v>1287</v>
       </c>
       <c r="D1299" s="64" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1300" s="10" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D1300" s="64" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1301" s="10" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D1301" s="64" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1302" s="10" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D1302" s="64" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="1303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1303" s="10" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D1303" s="64" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="1304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1304" s="10" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D1304" s="64" t="s">
         <v>1333</v>
@@ -19359,7 +19523,7 @@
     </row>
     <row r="1305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1305" s="10" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D1305" t="s">
         <v>1053</v>
@@ -19367,27 +19531,27 @@
     </row>
     <row r="1306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1306" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1307" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1309" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1310" s="10" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1311" s="10" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D1311" t="s">
         <v>1342</v>
@@ -19395,15 +19559,15 @@
     </row>
     <row r="1312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1312" s="10" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D1312" s="67" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1313" s="67" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1314" spans="1:4" x14ac:dyDescent="0.25">
@@ -19411,72 +19575,72 @@
         <v>1342</v>
       </c>
       <c r="D1314" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1315" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D1315" s="15" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1316" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D1316" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1317" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D1317" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1318" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D1318" s="67" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1319" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1320" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="1321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1321" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="1323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1323" t="s">
+        <v>1665</v>
+      </c>
+      <c r="D1323" t="s">
         <v>1666</v>
-      </c>
-      <c r="D1323" t="s">
-        <v>1667</v>
       </c>
     </row>
     <row r="1324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1324" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="1325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1325" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="1327" spans="1:4" x14ac:dyDescent="0.25">
@@ -19484,7 +19648,7 @@
         <v>43156</v>
       </c>
       <c r="B1327" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="1329" spans="1:4" x14ac:dyDescent="0.25">
@@ -19492,10 +19656,10 @@
         <v>43157</v>
       </c>
       <c r="B1329" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C1329" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D1329" t="s">
         <v>1342</v>
@@ -19503,10 +19667,10 @@
     </row>
     <row r="1330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1330" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D1330" s="15" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="1331" spans="1:4" x14ac:dyDescent="0.25">
@@ -19514,7 +19678,7 @@
         <v>990</v>
       </c>
       <c r="D1331" s="15" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="1332" spans="1:4" x14ac:dyDescent="0.25">
@@ -19522,31 +19686,31 @@
         <v>991</v>
       </c>
       <c r="D1332" s="15" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="1333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1333" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D1333" s="15" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="1334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1334" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D1334" s="15" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="1335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1335" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D1335" s="15" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="1336" spans="1:4" x14ac:dyDescent="0.25">
@@ -19556,17 +19720,17 @@
     </row>
     <row r="1337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1337" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="1338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1338" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="1339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1339" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D1339" t="s">
         <v>1053</v>
@@ -19574,26 +19738,26 @@
     </row>
     <row r="1340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1340" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="D1340" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="1341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1341" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D1341" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1342" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D1342" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="1343" spans="1:4" x14ac:dyDescent="0.25">
@@ -19601,44 +19765,44 @@
         <v>1342</v>
       </c>
       <c r="D1343" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="1344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1344" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D1344" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="1345" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1345" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D1345" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="1346" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1346" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="D1346" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1347" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1347" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D1347" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="1348" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1348" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D1348" t="s">
         <v>1052</v>
@@ -19646,39 +19810,39 @@
     </row>
     <row r="1349" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1349" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D1349" s="64" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1350" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1350" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D1350" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1351" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1351" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D1351" s="64" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="1352" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1352" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D1352" s="64" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="1353" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1353" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D1353" s="64" t="s">
         <v>1298</v>
@@ -19686,105 +19850,105 @@
     </row>
     <row r="1354" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1354" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D1354" s="64" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="1355" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1355" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="1356" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1356" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="1357" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1357" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="1361" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1361" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="1363" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1363" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="1364" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1364" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="1365" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1365" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="1366" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1366" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1367" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1367" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1368" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1368" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="1369" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1369" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="1370" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1370" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="1371" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1371" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="1372" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1372" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="1373" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1373" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="1374" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1374" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="1376" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1376" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="1378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1378" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="1379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1379" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="1382" spans="1:4" x14ac:dyDescent="0.25">
@@ -19792,10 +19956,10 @@
         <v>43158</v>
       </c>
       <c r="B1382" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1382" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D1382" t="s">
         <v>1052</v>
@@ -19803,136 +19967,136 @@
     </row>
     <row r="1383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1383" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D1383" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="1384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1384" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D1384" s="64" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="1385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1385" s="64" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1386" s="64" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1387" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D1387" s="64" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1388" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1389" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1391" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1392" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="1393" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1393" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="1394" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1394" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="1395" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1395" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="1396" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1396" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="1397" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1397" s="17" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="1398" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1398" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="1399" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1399" s="17" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="1404" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1404" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="1405" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1405" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="1406" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1406" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1408" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1408" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="1409" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C1409" s="3" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="1411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1411" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="1412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1412" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="1414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1414" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="1415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1415" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="1417" spans="1:3" x14ac:dyDescent="0.25">
@@ -19940,50 +20104,50 @@
         <v>43159</v>
       </c>
       <c r="C1417" s="69" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="1418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1418" s="69" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="1420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1420" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1420" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="1421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1421" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="1422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1422" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="1424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1424" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="1425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1425" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="1427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1427" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="1428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1428" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="1430" spans="1:4" x14ac:dyDescent="0.25">
@@ -19991,7 +20155,7 @@
         <v>1127</v>
       </c>
       <c r="C1430" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="1431" spans="1:4" x14ac:dyDescent="0.25">
@@ -19999,7 +20163,7 @@
         <v>1342</v>
       </c>
       <c r="C1431" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="1434" spans="1:4" x14ac:dyDescent="0.25">
@@ -20007,99 +20171,99 @@
         <v>43164</v>
       </c>
       <c r="B1434" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1434" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="1435" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1435" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="1436" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1436" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="1437" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1437" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="1438" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1438" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="1439" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1439" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="1440" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1440" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="C1440" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D1440" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="1441" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1441" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D1441" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="1442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1442" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="1443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1443" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="1444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1444" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="1445" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1445" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="1447" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1447" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="1448" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1448" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="1449" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1449" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="1450" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1450" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="1452" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1452" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="1454" spans="1:4" x14ac:dyDescent="0.25">
@@ -20107,69 +20271,69 @@
         <v>43165</v>
       </c>
       <c r="B1454" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="1455" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1455" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D1455" t="s">
         <v>1777</v>
-      </c>
-      <c r="D1455" t="s">
-        <v>1778</v>
       </c>
     </row>
     <row r="1456" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1456" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D1456" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1457" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1457" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="1459" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1459" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D1459" s="64" t="s">
         <v>1781</v>
-      </c>
-      <c r="D1459" s="64" t="s">
-        <v>1782</v>
       </c>
     </row>
     <row r="1460" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1460" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="1462" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1462" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="1463" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1463" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="1464" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1464" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="1465" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1465" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D1465" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1466" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1466" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="1469" spans="1:4" x14ac:dyDescent="0.25">
@@ -20177,53 +20341,53 @@
         <v>43166</v>
       </c>
       <c r="B1469" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1469" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="1470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1470" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="1471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1471" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="1472" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1472" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="1473" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1473" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="C1473" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="1474" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1474" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="1475" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1475" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="1476" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1476" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="1478" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1478" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="1479" spans="1:4" x14ac:dyDescent="0.25">
@@ -20231,10 +20395,10 @@
         <v>43167</v>
       </c>
       <c r="B1479" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1479" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="D1479" t="s">
         <v>1052</v>
@@ -20242,57 +20406,57 @@
     </row>
     <row r="1480" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1480" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D1480" s="64" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="1481" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1481" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="1482" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1482" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="1483" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1483" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D1483" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="1484" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1484" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="1485" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1485" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D1485" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="1486" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1486" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D1486" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="1487" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1487" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D1487" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="1489" spans="1:3" x14ac:dyDescent="0.25">
@@ -20300,68 +20464,68 @@
         <v>43168</v>
       </c>
       <c r="B1489" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C1489" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="1490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1490" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="1491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1491" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="1492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1492" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="1493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1493" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="1496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1496" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="C1496" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="1501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1501" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="1502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1502" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="1503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1503" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="1504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1504" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="1505" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1505" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="1507" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1507" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="1508" spans="1:4" x14ac:dyDescent="0.25">
@@ -20369,10 +20533,10 @@
         <v>43169</v>
       </c>
       <c r="B1508" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1508" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D1508" t="s">
         <v>1053</v>
@@ -20380,47 +20544,47 @@
     </row>
     <row r="1509" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1509" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D1509" s="10" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="1510" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1510" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D1510" s="10" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="1511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1511" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D1511" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="1512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1512" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D1512" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1513" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1513" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D1513" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="1514" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1514" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D1514" t="s">
         <v>1052</v>
@@ -20428,18 +20592,18 @@
     </row>
     <row r="1515" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1515" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D1515" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1516" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1516" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D1516" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="1517" spans="1:4" x14ac:dyDescent="0.25">
@@ -20447,36 +20611,36 @@
         <v>1287</v>
       </c>
       <c r="D1517" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1518" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1518" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D1518" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1519" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1519" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D1519" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="1520" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1520" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D1520" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="1521" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1521" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D1521" t="s">
         <v>1050</v>
@@ -20484,22 +20648,22 @@
     </row>
     <row r="1522" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1522" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="1523" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1523" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="1524" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1524" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="1525" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1525" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="1527" spans="1:4" x14ac:dyDescent="0.25">
@@ -20515,7 +20679,7 @@
         <v>43171</v>
       </c>
       <c r="B1528" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="1529" spans="1:4" x14ac:dyDescent="0.25">
@@ -20523,7 +20687,7 @@
         <v>43172</v>
       </c>
       <c r="B1529" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="1531" spans="1:4" x14ac:dyDescent="0.25">
@@ -20531,50 +20695,50 @@
         <v>43173</v>
       </c>
       <c r="C1531" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="1532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1532" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="1538" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1538" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="1539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1539" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="1540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1540" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="1541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1541" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="1542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1542" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="1544" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1544" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="C1544" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="1545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1545" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="1546" spans="1:3" x14ac:dyDescent="0.25">
@@ -20584,12 +20748,12 @@
     </row>
     <row r="1547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1547" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="1548" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1548" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="1551" spans="1:3" x14ac:dyDescent="0.25">
@@ -20597,40 +20761,40 @@
         <v>43176</v>
       </c>
       <c r="B1551" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C1551" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="1552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1552" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="1553" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1553" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="1554" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1554" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="1555" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1555" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="1556" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1556" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="1560" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1560" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="1562" spans="1:3" x14ac:dyDescent="0.25">
@@ -20646,7 +20810,7 @@
         <v>43178</v>
       </c>
       <c r="B1563" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="1564" spans="1:3" x14ac:dyDescent="0.25">
@@ -20654,135 +20818,135 @@
         <v>43179</v>
       </c>
       <c r="B1564" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="C1564" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="1565" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1565" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="1566" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1566" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="1567" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1567" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="1568" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1568" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="1569" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1569" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="1570" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1570" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="1571" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1571" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="1572" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1572" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="1573" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1573" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="1574" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1574" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="1575" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1575" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="1576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1576" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="1577" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1577" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="1578" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1578" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="1579" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1579" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1580" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1580" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="1581" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1581" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="1582" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1582" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="1583" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1583" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="1584" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1584" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="1585" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1585" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="1586" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1586" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1587" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1587" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="1588" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1588" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="1590" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1590" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="1593" spans="1:3" x14ac:dyDescent="0.25">
@@ -20790,65 +20954,65 @@
         <v>43180</v>
       </c>
       <c r="B1593" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1593" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="1594" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1594" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="1595" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1595" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="1596" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1596" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="1597" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1597" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="1598" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1598" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="1599" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1599" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="1600" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1600" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="1601" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1601" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="1602" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1602" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="1603" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1603" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1604" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1604" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="1607" spans="1:3" x14ac:dyDescent="0.25">
@@ -20856,71 +21020,71 @@
         <v>43181</v>
       </c>
       <c r="B1607" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="C1607" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="1608" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1608" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="1609" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1609" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="1610" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1610" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="1611" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1611" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="1614" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1614" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1614" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="1615" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1615" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="1618" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1618" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="C1618" s="73" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="1619" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1619" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="1620" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1620" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1621" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1621" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="1623" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1623" t="s">
-        <v>1921</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="1624" spans="1:4" x14ac:dyDescent="0.25">
@@ -20928,106 +21092,106 @@
         <v>43182</v>
       </c>
       <c r="B1624" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1624" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="D1624" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="1625" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1625" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="D1625" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1626" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1626" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="1627" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1627" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="1628" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1628" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="1629" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1629" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="C1629" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="1630" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1630" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="D1630" t="s">
-        <v>1928</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="1631" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1631" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="D1631" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="1632" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1632" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="D1632" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="1633" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1633" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="1635" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1635" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="1636" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1636" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="1637" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1637" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="1638" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1638" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="1639" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1639" t="s">
-        <v>1936</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="1640" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1640" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C1640" t="s">
-        <v>1937</v>
+        <v>1933</v>
       </c>
       <c r="D1640" t="s">
         <v>1332</v>
@@ -21035,38 +21199,41 @@
     </row>
     <row r="1641" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1641" t="s">
-        <v>1938</v>
+        <v>1934</v>
       </c>
       <c r="D1641" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="1642" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1642" t="s">
-        <v>1941</v>
+        <v>1937</v>
       </c>
       <c r="D1642" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1643" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1643" t="s">
-        <v>1944</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="1644" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1644" t="s">
-        <v>1939</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="1645" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1645" t="s">
-        <v>1940</v>
+        <v>1936</v>
+      </c>
+      <c r="D1645" t="s">
+        <v>1995</v>
       </c>
     </row>
     <row r="1646" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1646" t="s">
-        <v>1943</v>
+        <v>1939</v>
       </c>
       <c r="D1646" t="s">
         <v>1316</v>
@@ -21074,20 +21241,20 @@
     </row>
     <row r="1647" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C1647" t="s">
-        <v>1945</v>
+        <v>1941</v>
       </c>
       <c r="D1647" t="s">
-        <v>1942</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="1648" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D1648" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1649" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1649" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1650" spans="1:4" x14ac:dyDescent="0.25">
@@ -21095,68 +21262,403 @@
         <v>43183</v>
       </c>
       <c r="B1650" t="s">
-        <v>1946</v>
+        <v>1942</v>
       </c>
       <c r="C1650" t="s">
-        <v>1947</v>
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1656" t="s">
+        <v>1995</v>
       </c>
     </row>
     <row r="1657" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1657" t="s">
-        <v>1948</v>
+        <v>1944</v>
       </c>
       <c r="C1657" t="s">
-        <v>1949</v>
+        <v>1945</v>
+      </c>
+      <c r="D1657" t="s">
+        <v>1316</v>
       </c>
     </row>
     <row r="1658" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1658" t="s">
-        <v>1950</v>
+        <v>1946</v>
+      </c>
+      <c r="D1658" t="s">
+        <v>1956</v>
       </c>
     </row>
     <row r="1659" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1659" t="s">
-        <v>1953</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="1660" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1660" t="s">
-        <v>1951</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="1661" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1661" t="s">
-        <v>1954</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="1662" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1662" t="s">
-        <v>1952</v>
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1663" t="s">
+        <v>1997</v>
       </c>
     </row>
     <row r="1664" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1664" t="s">
+        <v>1951</v>
+      </c>
+      <c r="D1664" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1665" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D1665" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1666" t="s">
+        <v>1954</v>
+      </c>
+      <c r="D1666" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1667" t="s">
         <v>1955</v>
       </c>
-    </row>
-    <row r="1665" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1665" t="s">
-        <v>1956</v>
-      </c>
-    </row>
-    <row r="1666" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1666" t="s">
+      <c r="D1667" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1668" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1670" s="72">
+        <v>43184</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1671" s="72">
+        <v>43185</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C1671" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1672" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1673" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1674" s="73" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1675" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1676" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1677" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1678" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C1678" t="s">
         <v>1958</v>
       </c>
-    </row>
-    <row r="1667" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1667" t="s">
-        <v>1959</v>
-      </c>
-    </row>
-    <row r="1668" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1668" t="s">
-        <v>1957</v>
+      <c r="D1678" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1679" t="s">
+        <v>1964</v>
+      </c>
+      <c r="D1679" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1680" s="3" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D1680" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1681" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D1681" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1682" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D1682" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1683" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D1683" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1684" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D1684" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1685" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D1685" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C1686" s="3" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1688" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1690" s="72">
+        <v>43186</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C1690" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D1690" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1691" t="s">
+        <v>1979</v>
+      </c>
+      <c r="D1691" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1692" t="s">
+        <v>1980</v>
+      </c>
+      <c r="D1692" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1693" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D1693" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1694" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1695" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D1695" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1696" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D1696" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="1697" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1697" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1697" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1698" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1698" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D1698" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1699" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1699" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D1699" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="1700" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1700" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="1701" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1701" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="1702" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1702" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="1703" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1703" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="1704" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1704" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="1705" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1705" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D1705" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="1706" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1706" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D1706" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="1707" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1707" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D1707" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="1708" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1708" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="1709" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1709" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D1709" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="1710" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1710" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1710" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1711" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D1711" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1712" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1712" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="1713" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1713" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="1714" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1714" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="1715" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1715" t="s">
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
message: setting api changes of add sales-man and profession setting completed
</commit_message>
<xml_diff>
--- a/public/Documents/NewApiDoc(6-10).xlsx
+++ b/public/Documents/NewApiDoc(6-10).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="2014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="2083">
   <si>
     <t>Laravel Api(06-10-2016)               @Virat Sir</t>
   </si>
@@ -8770,10 +8770,217 @@
     <t xml:space="preserve"> igst problem state-city wise</t>
   </si>
   <si>
-    <t>Front-End(swaminarayan done)</t>
-  </si>
-  <si>
-    <t>Back-End(swaminarayan done)</t>
+    <t xml:space="preserve"> check : https://stackoverflow.com/questions/26346299/whats-the-correct-way-to-set-env-variables-in-laravel-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- client show/hide data from setting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     -- show/hide data of client in crm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Bill changes &gt;&gt; client insertion in bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     -- put design of plus button and open modal on click of plus button with all client show/hide data as per setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     -- make a call of client insert api and close the modal</t>
+  </si>
+  <si>
+    <t>app\views\PopupModal\Client</t>
+  </si>
+  <si>
+    <t>app\js\controllers\PopupModal\Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uploading to server of arihant,swaminarayan and testing properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Git push files of front-end as well as back-end</t>
+  </si>
+  <si>
+    <t>app\js\controllers\Accounting\viewData\AccViewCtrl.js</t>
+  </si>
+  <si>
+    <t>stock-summary &gt;&gt; product color-size hiding pending</t>
+  </si>
+  <si>
+    <t>app\views\CRM\Client\CrmClientFilterData.html</t>
+  </si>
+  <si>
+    <t>Back-End(arihant done,swaminarayan done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> client update model show- hide data</t>
+  </si>
+  <si>
+    <t>Front-End(arihant done,swaminarayan done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Question Discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Filed add credit limit and credit days in client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. change date period</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. implementation of igst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4. Add Salesman </t>
+  </si>
+  <si>
+    <t>Analysis on today working points and discuss it</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solve the problem of bill insertion &gt;&gt; this problem occur after client-data disable(for state-city) as per setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LedgerTransformer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BillProcessor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BillTransformer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Database Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- solution : remove foreign key of state-city from ledger and convert undefined state-city to null by checking the value in sale-bill and ledger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- problem solve of cant display data on click of previous button in sale-bill (problem of 'reduce' predefined function in angularjs)</t>
+  </si>
+  <si>
+    <t>Attend Client Call</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- explain working of quick-menu of product</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- explain +/- button in expense in bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     --change caption in quick bill &gt;&gt; From sale-invoice/sale-purchase to tax-sale/tax-purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Changes </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> try to solve the problem product data not loading after updating it in angularjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- client model update &gt;&gt; add show-hide client data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- stock-summary &gt;&gt; add show-hide product color-size </t>
+  </si>
+  <si>
+    <t>app\views\Inventory\StockSummary\InvStockSummary.html</t>
+  </si>
+  <si>
+    <t>app\js\controllers\Inventory\StockSummary\InvStockSummaryCtrl.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> change the design of client-modal (looks awkward when we show-hide client data)</t>
+  </si>
+  <si>
+    <t>app\views\PopupModal\CRM\ClientForm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solve the problem of sending message from admin to all other admin and teacher to all admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> make new api &gt;&gt; Send message "Admin to Teacher (Line#60 Point#38)" need teacher list from gradeId and sectionId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> make new api &gt;&gt; Send message "Teacher to single Admin (Line#133 Point#86)" need admin list</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> change the design of sale-bill and quotation (looks awkward when we show-hide client data) (time consuming)</t>
+  </si>
+  <si>
+    <t>ERP(Arihant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5. display all ledger with its current balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> display all ledger with its current balance</t>
+  </si>
+  <si>
+    <t>app\js\controllers\Accounting\Ledger\LedgerCtrl.js</t>
+  </si>
+  <si>
+    <t>app\views\Accounting\Ledger\Ledger.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> problem solve of cant get message from app (admin to teacher)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Extra &gt;&gt; found that cant save data properly when sending message from app to web</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pragnesh point</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1. Admin:: Web to Mobile App - Admin to All Parents of One Section (Line#26 Point#15) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Admin:: Web to Mobile App - Admin to All Parents of school (Line#28 Point#17) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3. check point &gt;&gt; send message to all section from admin to parent(Point#7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ERP(arihant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Setting Option Changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- add setting of profession in client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Front-End &amp; Back-End Changes In Setting(manual,design,get-set data,api changes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- add setting of salesman required/not in bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Add credit-limit and credit-days in client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Front-End </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- design change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- insert,update and set data in client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- api(insert,update,get all data,get particular data) changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Crm &gt;&gt; client-update model changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bill api changes(add salesman)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- insert,update and set data in bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setting api changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> constantclass.php</t>
   </si>
 </sst>
 </file>
@@ -9230,7 +9437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -9323,9 +9530,11 @@
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9335,9 +9544,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -11884,10 +12090,10 @@
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A409" s="74" t="s">
+      <c r="A409" s="75" t="s">
         <v>852</v>
       </c>
-      <c r="B409" s="74"/>
+      <c r="B409" s="75"/>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
@@ -12013,18 +12219,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1715"/>
+  <dimension ref="A1:I1785"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1701" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1705" sqref="D1705"/>
+    <sheetView tabSelected="1" topLeftCell="C1759" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1765" sqref="D1765"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="111.7109375" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="125.42578125" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" customWidth="1"/>
     <col min="5" max="5" width="75.5703125" customWidth="1"/>
     <col min="6" max="6" width="114.85546875" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
@@ -17003,7 +17209,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="825" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C825" s="60" t="s">
         <v>1228</v>
       </c>
@@ -17976,7 +18182,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="1006" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1006" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1006" s="3" t="s">
         <v>1389</v>
       </c>
@@ -21524,6 +21730,9 @@
       </c>
     </row>
     <row r="1695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1695" t="s">
+        <v>1533</v>
+      </c>
       <c r="C1695" t="s">
         <v>2010</v>
       </c>
@@ -21596,7 +21805,7 @@
         <v>2003</v>
       </c>
       <c r="D1705" t="s">
-        <v>2013</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="1706" spans="3:4" x14ac:dyDescent="0.25">
@@ -21619,46 +21828,474 @@
       <c r="C1708" t="s">
         <v>2004</v>
       </c>
+      <c r="D1708" t="s">
+        <v>1710</v>
+      </c>
     </row>
     <row r="1709" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1709" t="s">
         <v>2005</v>
       </c>
-      <c r="D1709" t="s">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="1710" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C1710" t="s">
-        <v>2009</v>
-      </c>
-      <c r="D1710" t="s">
-        <v>1425</v>
-      </c>
     </row>
     <row r="1711" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D1711" t="s">
-        <v>1466</v>
+      <c r="C1711" t="s">
+        <v>2013</v>
       </c>
     </row>
     <row r="1712" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C1712" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="1713" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1713" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D1713" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="1714" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1714" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D1714" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1715" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1715" t="s">
+        <v>2016</v>
+      </c>
+      <c r="D1715" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1716" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1716" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D1716" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="1717" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1717" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D1717" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1718" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1718" t="s">
+        <v>2021</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="1719" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1719" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1720" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D1720" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="1721" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1721" s="47" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="1713" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1713" t="s">
+      <c r="D1721" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="1722" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1722" s="47" t="s">
         <v>1977</v>
       </c>
-    </row>
-    <row r="1714" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1714" t="s">
+      <c r="D1722" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="1723" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1723" s="47" t="s">
         <v>1978</v>
       </c>
     </row>
-    <row r="1715" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1715" t="s">
+    <row r="1724" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1724" s="47" t="s">
         <v>2011</v>
+      </c>
+    </row>
+    <row r="1725" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1725" s="47" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="1726" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1726" s="47" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="1727" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C1727" s="47" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1729" s="72">
+        <v>43187</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C1729" s="10" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1730" s="10" t="s">
+        <v>2029</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1731" s="10" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1732" s="10" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1733" s="10" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1734" s="76" t="s">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1737" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1738" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1739" t="s">
+        <v>2039</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1740" t="s">
+        <v>2040</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1741" t="s">
+        <v>2041</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1742" t="s">
+        <v>2042</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1743" t="s">
+        <v>2043</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1744" t="s">
+        <v>2045</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1745" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1746" t="s">
+        <v>2046</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1747" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1748" s="10" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1749" s="10" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1750" s="10" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1751" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1752" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:4" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1753" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1754" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1755" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1756" t="s">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1758" s="72">
+        <v>43188</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C1758" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1759" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1760" t="s">
+        <v>2066</v>
+      </c>
+    </row>
+    <row r="1761" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1761" t="s">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="1763" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1763" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C1763" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D1763" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="1764" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1764" t="s">
+        <v>2071</v>
+      </c>
+      <c r="D1764" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="1765" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1765" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D1765" t="s">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="1766" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1766" t="s">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="1767" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1767" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="1768" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1768" t="s">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="1769" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1769" t="s">
+        <v>2075</v>
+      </c>
+      <c r="D1769" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1770" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1770" t="s">
+        <v>2076</v>
+      </c>
+      <c r="D1770" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1771" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1771" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D1771" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1772" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1772" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1773" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1773" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1774" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1774" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="1775" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1775" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1776" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C1776" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="1777" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1777" t="s">
+        <v>2078</v>
+      </c>
+    </row>
+    <row r="1778" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1778" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="1779" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1779" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1780" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1780" t="s">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="1781" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1781" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="1782" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1782" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="1783" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1783" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="1784" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1784" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="1785" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1785" t="s">
+        <v>2077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>